<commit_message>
Dang ky by mrdat 27/05/2021
</commit_message>
<xml_diff>
--- a/Internfinder-BE/GAO_BackEnd/src/main/resources/jxls/template-CV.xlsx
+++ b/Internfinder-BE/GAO_BackEnd/src/main/resources/jxls/template-CV.xlsx
@@ -328,7 +328,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CV59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23:BA30"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BP8" sqref="BP8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.88671875" defaultRowHeight="13.5" customHeight="1"/>

</xml_diff>